<commit_message>
add key file & update expenses
</commit_message>
<xml_diff>
--- a/expense_for_tax_return.xlsx
+++ b/expense_for_tax_return.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\204027647\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\204027647\github\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8B8286-9FF1-4584-9651-8D95F6A3CCB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997CAE43-6073-420E-9CED-0BF4ECE3ED08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="610" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="285">
   <si>
     <t>Golf Club</t>
   </si>
@@ -926,6 +926,15 @@
   </si>
   <si>
     <t>Brevard School Foundation</t>
+  </si>
+  <si>
+    <t>water heater</t>
+  </si>
+  <si>
+    <t>1+1+1</t>
+  </si>
+  <si>
+    <t>Edgewood</t>
   </si>
 </sst>
 </file>
@@ -1790,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A62" zoomScale="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView view="pageLayout" topLeftCell="A59" zoomScale="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2563,7 +2572,7 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A50" zoomScale="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3137,6 +3146,12 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>282</v>
+      </c>
+      <c r="B60">
+        <v>875</v>
+      </c>
       <c r="C60" t="s">
         <v>276</v>
       </c>
@@ -3161,16 +3176,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="1" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="12.6328125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="25.6328125" customWidth="1"/>
@@ -3373,11 +3387,33 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B22">
+        <v>350</v>
+      </c>
       <c r="C22" t="s">
         <v>238</v>
       </c>
       <c r="D22" t="s">
         <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3387,10 +3423,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A100" zoomScale="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A101" zoomScale="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4231,7 +4267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>188</v>
       </c>
@@ -4239,20 +4275,26 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>89</v>
       </c>
       <c r="B98">
         <v>50</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
+        <v>284</v>
+      </c>
+      <c r="D98">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2020</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>185</v>
       </c>
@@ -4260,7 +4302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>244</v>
       </c>
@@ -4268,7 +4310,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>274</v>
       </c>
@@ -4276,7 +4318,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>189</v>
       </c>
@@ -4284,7 +4326,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>279</v>
       </c>
@@ -4295,12 +4337,20 @@
         <v>280</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>281</v>
       </c>
       <c r="B105">
         <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>259</v>
+      </c>
+      <c r="B106">
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -4539,8 +4589,8 @@
       <c r="A2">
         <v>2020</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>